<commit_message>
Added Requirements and mapping
Functional requirements, non-functional requirements have been added in the Specific Requirements section of Matteo Biasielli's file. Moreover, they have been mapped into goals and a few of them have been justified.
Updated effort spent and GANTT table
</commit_message>
<xml_diff>
--- a/RASD/GANTT.xlsx
+++ b/RASD/GANTT.xlsx
@@ -90,7 +90,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -109,6 +109,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -122,7 +128,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -130,6 +136,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -434,7 +441,7 @@
   <dimension ref="A1:W9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,8 +545,8 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">

</xml_diff>

<commit_message>
updated general RASD file
merged Mattia's and Matteo's work
</commit_message>
<xml_diff>
--- a/RASD/GANTT.xlsx
+++ b/RASD/GANTT.xlsx
@@ -470,7 +470,7 @@
   <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="J6" sqref="J6:N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,14 +685,14 @@
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="3"/>
+      <c r="H11" s="8"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="C12" s="10"/>

</xml_diff>

<commit_message>
Added UI to the general RASD file
Minor changes on the Cladd diagram description and the use cases diagram description. Updated GANTT
</commit_message>
<xml_diff>
--- a/RASD/GANTT.xlsx
+++ b/RASD/GANTT.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>What</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Alloy</t>
   </si>
   <si>
-    <t>??</t>
-  </si>
-  <si>
     <t>Complete revision</t>
   </si>
   <si>
@@ -72,6 +69,9 @@
   </si>
   <si>
     <t>Emilio*</t>
+  </si>
+  <si>
+    <t>Software System Attributes</t>
   </si>
 </sst>
 </file>
@@ -154,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -166,6 +166,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -470,7 +471,7 @@
   <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,7 +610,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="3"/>
@@ -679,22 +680,35 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -702,9 +716,9 @@
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
       <c r="M12" s="9"/>
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>

</xml_diff>

<commit_message>
Missing UIs + Travlendar logo
Minor updates to GANTT and RASD.
</commit_message>
<xml_diff>
--- a/RASD/GANTT.xlsx
+++ b/RASD/GANTT.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="432" windowWidth="20736" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>What</t>
   </si>
@@ -72,12 +72,15 @@
   </si>
   <si>
     <t>Software System Attributes</t>
+  </si>
+  <si>
+    <t>User Interfaces description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -116,7 +119,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,6 +144,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -154,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -167,6 +176,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -176,6 +186,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -468,26 +481,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W12"/>
+  <dimension ref="A1:W13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.44140625" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
     <col min="4" max="8" width="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="15" width="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.109375" bestFit="1" customWidth="1"/>
     <col min="17" max="22" width="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="3.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -558,22 +571,23 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -583,7 +597,7 @@
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -593,7 +607,7 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -605,7 +619,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -613,19 +627,19 @@
         <v>15</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -645,7 +659,7 @@
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -656,7 +670,7 @@
       <c r="H8" s="10"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -675,7 +689,7 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -693,7 +707,7 @@
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -702,7 +716,7 @@
       </c>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -731,6 +745,19 @@
       <c r="V12" s="9"/>
       <c r="W12" s="9"/>
     </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -743,7 +770,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -755,7 +782,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated GANTT and RASD
updated UI on RASD, that still need descriptions
</commit_message>
<xml_diff>
--- a/RASD/GANTT.xlsx
+++ b/RASD/GANTT.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="432" windowWidth="20736" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>What</t>
   </si>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -163,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -175,7 +175,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -481,23 +480,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W13"/>
+  <dimension ref="A1:W14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+      <selection activeCell="AA10" sqref="AA10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.44140625" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
     <col min="4" max="8" width="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="15" width="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="22" width="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="3.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
@@ -627,13 +626,13 @@
         <v>15</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
@@ -705,7 +704,7 @@
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
+      <c r="Q10" s="2"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -730,9 +729,9 @@
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
       <c r="M12" s="9"/>
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>
@@ -757,6 +756,15 @@
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P14" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -770,7 +778,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -782,7 +790,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>